<commit_message>
Update content of toolbox and descriptions
</commit_message>
<xml_diff>
--- a/orthomyxoviruses/family.xlsx
+++ b/orthomyxoviruses/family.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Human Influenza A/H3N2</t>
+          <t>A/H3N2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -544,24 +544,44 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>H3N8</t>
+          <t>H7N9</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>H3N8</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>H7N9</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A/H7N9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Avian influenza (Bird Flu)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -572,24 +592,44 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H4N6</t>
+          <t>Victoria</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H4N6</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>B/Victoria</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>B/Victoria</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Flu</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Influenza (Flu)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Influenza B</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -600,24 +640,44 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>H14N3</t>
+          <t>Yamagata</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>H14N3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+          <t>B/Yamagata</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>B/Yamagata</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Flu</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Influenza (Flu)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Influenza B</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -628,27 +688,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>H7N9</t>
+          <t>H1N1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>H7N9</t>
+          <t>H1N1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Avian influenza A/H7N9</t>
+          <t>A/H1N1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Flu</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Avian influenza (Bird Flu)</t>
+          <t>Influenza (Flu)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -676,24 +736,44 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>H15N9</t>
+          <t>H5N1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>H15N9</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+          <t>H5N1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A/H5N1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Avian influenza (Bird Flu)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -704,24 +784,44 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>H10N7</t>
+          <t>H9N2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>H10N7</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+          <t>H9N2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A/H9N2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Avian influenza (Bird Flu)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -732,32 +832,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>H3N8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>B/Victoria</t>
+          <t>H3N8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Human influenza B/Victoria</t>
+          <t>A/H3N8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Flu</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Influenza (Flu)</t>
+          <t>Avian influenza (Bird Flu)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Influenza B</t>
+          <t>Influenza A</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -780,32 +880,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Yamagata</t>
+          <t>H4N6</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>B/Yamagata</t>
+          <t>H4N6</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Human influenza B/Yamagata</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Flu</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Influenza (Flu)</t>
-        </is>
-      </c>
+          <t>A/H4N6</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Influenza B</t>
+          <t>Influenza A</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -815,7 +907,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -828,29 +920,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>H1N1</t>
+          <t>H14N3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>H1N1</t>
+          <t>H14N3</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Human influenza A/H1N1</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Flu</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Influenza (Flu)</t>
-        </is>
-      </c>
+          <t>A/H14N3</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
           <t>Influenza A</t>
@@ -863,7 +947,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -876,24 +960,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>H2N2</t>
+          <t>H15N9</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>H2N2</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>H15N9</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>A/H15N9</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -904,29 +1000,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>H5N1</t>
+          <t>H10N7</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>H5N1</t>
+          <t>H10N7</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Avian influenza A/H5N1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>AI</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Avian influenza (Bird Flu)</t>
-        </is>
-      </c>
+          <t>A/H10N7</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>Influenza A</t>
@@ -939,7 +1027,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -952,24 +1040,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>H6N2</t>
+          <t>H2N2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>H6N2</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
+          <t>H2N2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>A/H2N2</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -980,24 +1080,36 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>H17N10</t>
+          <t>H6N2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>H17N10</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+          <t>H6N2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>A/H6N2</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1008,24 +1120,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>H18N11</t>
+          <t>H17N10</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>H18N11</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
+          <t>H17N10</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>A/H17N10</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -1036,24 +1160,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>H8N4</t>
+          <t>H18N11</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>H8N4</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>H18N11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>A/H18N11</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1064,29 +1200,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>H9N2</t>
+          <t>H8N4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>H9N2</t>
+          <t>H8N4</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Avian influenza H9N2</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>AI</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Avian influenza (Bird Flu)</t>
-        </is>
-      </c>
+          <t>A/H8N4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>Influenza A</t>
@@ -1099,7 +1227,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1120,16 +1248,28 @@
           <t>H11N9</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>A/H11N9</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -1148,16 +1288,28 @@
           <t>H12N5</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>A/H12N5</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1176,16 +1328,28 @@
           <t>H13N6</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>A/H13N6</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1204,16 +1368,28 @@
           <t>H16N3</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>A/H16N3</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Influenza A</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>

</xml_diff>

<commit_message>
Use acronyms instead of full names in tabsets
</commit_message>
<xml_diff>
--- a/orthomyxoviruses/family.xlsx
+++ b/orthomyxoviruses/family.xlsx
@@ -516,7 +516,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Influenza (Flu)</t>
+          <t>Influenza</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Influenza (Flu)</t>
+          <t>Influenza</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -660,7 +660,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Influenza (Flu)</t>
+          <t>Influenza</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Influenza (Flu)</t>
+          <t>Influenza</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">

</xml_diff>